<commit_message>
Mapping: new classes added
</commit_message>
<xml_diff>
--- a/05_Implementation/PoC/Mapping TED XML to ePO.xlsx
+++ b/05_Implementation/PoC/Mapping TED XML to ePO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="121">
   <si>
     <t>ePO TTL</t>
   </si>
@@ -242,13 +242,154 @@
   <si>
     <t xml:space="preserve">If CONTRACTING_BODY/JOINT_PROCUREMENT_INVOLVED, jointProcurement with each of the
 CONTRACTING_BODY/ADDRESS_CONTRACTING_BODY_ADDITIONAL </t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>Criterion</t>
+  </si>
+  <si>
+    <t>ExpressionOfInterest</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>AccountFormat</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>BuyerCategoryType</t>
+  </si>
+  <si>
+    <t>BuyerRoleType</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>EOGroupCodeType</t>
+  </si>
+  <si>
+    <t>IdentifierProvider</t>
+  </si>
+  <si>
+    <t>LegalForm</t>
+  </si>
+  <si>
+    <t>ProcedureChoiceJustificationCode</t>
+  </si>
+  <si>
+    <t>ProcedureType</t>
+  </si>
+  <si>
+    <t>ProcuringEntityRoleType</t>
+  </si>
+  <si>
+    <t>ProcuringEntityType</t>
+  </si>
+  <si>
+    <t>ReservedContract</t>
+  </si>
+  <si>
+    <t>ReservedContractType</t>
+  </si>
+  <si>
+    <t>SubmissionLanguage</t>
+  </si>
+  <si>
+    <t>TenderingCriterion</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>ProcurementDocument</t>
+  </si>
+  <si>
+    <t>CallForCompetition</t>
+  </si>
+  <si>
+    <t>CallForProposal</t>
+  </si>
+  <si>
+    <t>CallForTenders</t>
+  </si>
+  <si>
+    <t>InvitationToTender</t>
+  </si>
+  <si>
+    <t>Notice</t>
+  </si>
+  <si>
+    <t>ContractAwardNotice</t>
+  </si>
+  <si>
+    <t>ContractNotice</t>
+  </si>
+  <si>
+    <t>PriorInformationNotice</t>
+  </si>
+  <si>
+    <t>TechnicalSpecifications</t>
+  </si>
+  <si>
+    <t>TenderDocument</t>
+  </si>
+  <si>
+    <t>FinancialTender</t>
+  </si>
+  <si>
+    <t>TechnicalTender</t>
+  </si>
+  <si>
+    <t>FundsIdentification</t>
+  </si>
+  <si>
+    <t>Lot</t>
+  </si>
+  <si>
+    <t>ServiceProvider</t>
+  </si>
+  <si>
+    <t>Tender</t>
+  </si>
+  <si>
+    <t>TenderingTerms</t>
+  </si>
+  <si>
+    <t>TenderShortList</t>
+  </si>
+  <si>
+    <t>Buyer - org:Organization/Buyer</t>
+  </si>
+  <si>
+    <t>ProcuringEntity - org:Organization/ProcuringEntity</t>
+  </si>
+  <si>
+    <t>EconomicOperator - regorg:RegisteredOrganization/EconomicOperator</t>
+  </si>
+  <si>
+    <t>EconomicOperatorGroup - regorg:RegisteredOrganization/EconomicOperatorGroup</t>
+  </si>
+  <si>
+    <t>RegisteredOrganization - regorg:RegisteredOrganization</t>
+  </si>
+  <si>
+    <t>ProcurementProcedure -  - ProcurementProject/ProcurementProcedure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,14 +406,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,13 +413,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -301,9 +461,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -316,18 +475,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,7 +512,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -632,24 +798,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D14"/>
+  <dimension ref="B2:D56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="51.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="76.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="60.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -660,69 +828,282 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>5</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" t="s">
         <v>67</v>
       </c>
     </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="B2:B56">
+    <sortCondition ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -732,458 +1113,462 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="51.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="84.28515625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="3.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="84.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="F2" s="5" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="F26" s="9" t="s">
+      <c r="D26" s="2"/>
+      <c r="F26" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E40" s="7"/>
+      <c r="E40" s="4"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="4" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Questions related to ProcruingEntity transformation
</commit_message>
<xml_diff>
--- a/05_Implementation/PoC/Mapping TED XML to ePO.xlsx
+++ b/05_Implementation/PoC/Mapping TED XML to ePO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7050"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="127">
   <si>
     <t>ePO TTL</t>
   </si>
@@ -233,9 +233,6 @@
     <t>hasMainActivity</t>
   </si>
   <si>
-    <t>Should be the same code list as TED XSD? (value: DEFENCE, ECONOMIC_AND_FINANCIAL_AFFAIRS, EDUCATION, ENVIRONMENT, GENERAL_PUBLIC_SERVICES, HEALTH, HOUSING_AND_COMMUNITY_AMENITIES, PUBLIC_ORDER_AND_SAFETY, RECREATION_CULTURE_AND_RELIGION, SOCIAL_PROTECTION)</t>
-  </si>
-  <si>
     <t>If CONTRACTING_BODY/JOINT_PROCUREMENT_INVOLVED, then current RoleType = Joint Procurement Lead,
 Other CONTRACTING_BODY/ADDRESS_CONTRACTING_BODY_ADDITIONAL RoleType = Joint Procurement Member.</t>
   </si>
@@ -386,13 +383,31 @@
   </si>
   <si>
     <t>URL_BUYER</t>
+  </si>
+  <si>
+    <t>Comments during the implementation</t>
+  </si>
+  <si>
+    <t>To do once the CM is updated.</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>F20 does not have CA_ACTIVITY nor CE_ACTIVITY defined.</t>
+  </si>
+  <si>
+    <t>Should be the same code list as TED XSD? CONTRACTING_BODY/CE_ACTIVITY or CA_ACTIVITY</t>
+  </si>
+  <si>
+    <t>Joint procurement / Procuring entity, which Procuring Entity type have?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,6 +446,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -464,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -497,6 +519,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,7 +543,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -803,11 +831,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="76.5703125" bestFit="1" customWidth="1"/>
@@ -831,22 +859,22 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -854,72 +882,72 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D21" t="s">
         <v>66</v>
@@ -927,7 +955,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D22" t="s">
         <v>67</v>
@@ -935,12 +963,12 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -950,12 +978,12 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -965,32 +993,32 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -1000,27 +1028,27 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
@@ -1030,7 +1058,7 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D42" t="s">
         <v>65</v>
@@ -1038,72 +1066,72 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1117,13 +1145,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F41"/>
+  <dimension ref="B2:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1131,10 +1159,11 @@
     <col min="4" max="4" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="84.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="45.5703125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1144,8 +1173,11 @@
       <c r="F2" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
@@ -1158,7 +1190,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1169,7 +1201,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1180,7 +1212,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1191,7 +1223,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1202,7 +1234,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1213,7 +1245,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1224,7 +1256,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1235,7 +1267,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1246,7 +1278,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1257,7 +1289,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1268,7 +1300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1279,7 +1311,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1290,7 +1322,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1298,7 +1330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1306,7 +1338,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1317,7 +1349,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1328,7 +1360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
@@ -1339,7 +1371,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1350,7 +1382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1361,18 +1393,21 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="12" t="s">
         <v>46</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G23" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1383,10 +1418,13 @@
         <v>47</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1399,20 +1437,24 @@
       <c r="F25" s="6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="G25" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="12" t="s">
         <v>70</v>
       </c>
       <c r="D26" s="2"/>
-      <c r="F26" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F26" s="6"/>
+      <c r="G26" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
@@ -1423,10 +1465,13 @@
         <v>38</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>9</v>
       </c>
@@ -1434,7 +1479,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>10</v>
       </c>
@@ -1445,7 +1490,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>10</v>
       </c>
@@ -1456,7 +1501,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>10</v>
       </c>
@@ -1467,7 +1512,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Remove code as classes
</commit_message>
<xml_diff>
--- a/05_Implementation/PoC/Mapping TED XML to ePO.xlsx
+++ b/05_Implementation/PoC/Mapping TED XML to ePO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="120">
   <si>
     <t>ePO TTL</t>
   </si>
@@ -244,55 +244,10 @@
     <t>ExpressionOfInterest</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>AccountFormat</t>
-  </si>
-  <si>
-    <t>AccountType</t>
-  </si>
-  <si>
-    <t>BuyerCategoryType</t>
-  </si>
-  <si>
-    <t>BuyerRoleType</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>EOGroupCodeType</t>
-  </si>
-  <si>
-    <t>IdentifierProvider</t>
-  </si>
-  <si>
-    <t>LegalForm</t>
-  </si>
-  <si>
-    <t>ProcedureChoiceJustificationCode</t>
-  </si>
-  <si>
-    <t>ProcedureType</t>
-  </si>
-  <si>
     <t>ProcuringEntityRoleType</t>
   </si>
   <si>
     <t>ProcuringEntityType</t>
-  </si>
-  <si>
-    <t>ReservedContract</t>
-  </si>
-  <si>
-    <t>ReservedContractType</t>
-  </si>
-  <si>
-    <t>SubmissionLanguage</t>
   </si>
   <si>
     <t>TenderingCriterion</t>
@@ -853,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D56"/>
+  <dimension ref="B2:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,279 +838,199 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>76</v>
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>71</v>
+        <v>99</v>
+      </c>
+      <c r="D14" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+      <c r="D15" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>82</v>
+        <v>98</v>
+      </c>
+      <c r="D29" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1171,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,7 +1073,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -1428,7 +1303,7 @@
         <v>37</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="60" x14ac:dyDescent="0.25">
@@ -1445,7 +1320,7 @@
         <v>69</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="75" x14ac:dyDescent="0.25">
@@ -1462,7 +1337,7 @@
         <v>67</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1475,7 +1350,7 @@
       <c r="D26" s="2"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1492,7 +1367,7 @@
         <v>70</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -1555,7 +1430,7 @@
         <v>4</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
@@ -1569,7 +1444,7 @@
         <v>57</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
@@ -1583,7 +1458,7 @@
         <v>6</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -1597,7 +1472,7 @@
         <v>54</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -1622,10 +1497,10 @@
         <v>52</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -1647,13 +1522,13 @@
         <v>12</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
@@ -1668,7 +1543,7 @@
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="1" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
@@ -1682,7 +1557,7 @@
         <v>64</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mapping updated: Call for Competition, Call for Tenders, Call for Proposal
</commit_message>
<xml_diff>
--- a/05_Implementation/PoC/Mapping TED XML to ePO.xlsx
+++ b/05_Implementation/PoC/Mapping TED XML to ePO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="193">
   <si>
     <t>ePO TTL</t>
   </si>
@@ -608,6 +608,12 @@
   </si>
   <si>
     <t>- Reserved contract depends on: LEFTI/RESTRICTED_SHELTERED_WORKSHOP or RESTRICTED_SHELTERED_PROGRAM</t>
+  </si>
+  <si>
+    <t>PRI_CALL_COMPETITION (PIN type)/D_PROC_NEGOTIATED_PRIOR_CALL_COMPETITION (common xsd)</t>
+  </si>
+  <si>
+    <t>Not found in TED</t>
   </si>
 </sst>
 </file>
@@ -723,7 +729,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -766,6 +772,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,7 +825,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1106,16 +1113,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="76.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="87.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="90.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
@@ -1151,19 +1158,29 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>77</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>78</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>79</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -1448,11 +1465,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G42"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E15"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1976,7 +1993,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Economic Operator as Winner mapping
</commit_message>
<xml_diff>
--- a/05_Implementation/PoC/Mapping TED XML to ePO.xlsx
+++ b/05_Implementation/PoC/Mapping TED XML to ePO.xlsx
@@ -12,12 +12,15 @@
     <sheet name="TED XSD" sheetId="3" r:id="rId3"/>
     <sheet name="TED to ePO" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Classes!$B$2:$D$57</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="249">
   <si>
     <t>ePO TTL</t>
   </si>
@@ -52,9 +55,6 @@
     <t>regorg:RegisteredOrganization/EconomicOperator</t>
   </si>
   <si>
-    <t>regorg:RegisteredOrganization/EconomicOperatorGroup</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
@@ -172,22 +172,10 @@
     <t>hasQualifyingParty</t>
   </si>
   <si>
-    <t>isMemberOf</t>
-  </si>
-  <si>
     <t>isSubcontractedBy</t>
   </si>
   <si>
     <t>subcontracts</t>
-  </si>
-  <si>
-    <t>groupsEconomicOperators</t>
-  </si>
-  <si>
-    <t>hasEOGroupCodeType</t>
-  </si>
-  <si>
-    <t>EO Group code</t>
   </si>
   <si>
     <t>CONTRACTING_BODY</t>
@@ -276,12 +264,6 @@
     <t>ProcuringEntity - org:Organization/ProcuringEntity</t>
   </si>
   <si>
-    <t>EconomicOperator - regorg:RegisteredOrganization/EconomicOperator</t>
-  </si>
-  <si>
-    <t>EconomicOperatorGroup - regorg:RegisteredOrganization/EconomicOperatorGroup</t>
-  </si>
-  <si>
     <t>RegisteredOrganization - regorg:RegisteredOrganization</t>
   </si>
   <si>
@@ -303,9 +285,6 @@
     <t>AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTOR[1..N] and AWARDED_TO_GROUP</t>
   </si>
   <si>
-    <t>EOPrepares</t>
-  </si>
-  <si>
     <t>ePO does not have values for this code list</t>
   </si>
   <si>
@@ -318,13 +297,7 @@
     <t>AWARD_CONTRACT/AWARDED_CONTRACT/LIKELY_SUBCONTRACTED exists, EO subcontracted might be INFO_ADD_SUBCONTRACTING as text.</t>
   </si>
   <si>
-    <t>Each AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTOR</t>
-  </si>
-  <si>
     <t>This info does not exist in TED XSD</t>
-  </si>
-  <si>
-    <t>AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTOR if NO_AWARDED_TO_GROUP</t>
   </si>
   <si>
     <t>NOTICE</t>
@@ -736,6 +709,96 @@
   </si>
   <si>
     <t>Fax/vCard:hasValue</t>
+  </si>
+  <si>
+    <t>Tenderer</t>
+  </si>
+  <si>
+    <t>Winner / EconomicOperator - regorg:RegisteredOrganization/EconomicOperator</t>
+  </si>
+  <si>
+    <t>group of</t>
+  </si>
+  <si>
+    <t>AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTOR if AWARDED_TO_GROUP</t>
+  </si>
+  <si>
+    <t>hasEOIndustryClassification</t>
+  </si>
+  <si>
+    <t>EO Industry Classification</t>
+  </si>
+  <si>
+    <t>SME if AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTOR/SME, LARGE if AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTOR/NO_SME</t>
+  </si>
+  <si>
+    <t>regorg:RegisteredOrganization/EconomicOperator as Winner</t>
+  </si>
+  <si>
+    <t>Winner</t>
+  </si>
+  <si>
+    <t>hasWinnerRank</t>
+  </si>
+  <si>
+    <t>Numeric</t>
+  </si>
+  <si>
+    <t>regorg:RegisteredOrganization</t>
+  </si>
+  <si>
+    <t>hasLegalName</t>
+  </si>
+  <si>
+    <t>AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTOR/ADDRESS_CONTRACTOR/OFFICIALNAME</t>
+  </si>
+  <si>
+    <t>adms:Identifier</t>
+  </si>
+  <si>
+    <t>rov:registration</t>
+  </si>
+  <si>
+    <t>AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTOR/ADDRESS_CONTRACTOR/NATIONALID</t>
+  </si>
+  <si>
+    <t>org:hasRegisteredSite</t>
+  </si>
+  <si>
+    <t>vCard</t>
+  </si>
+  <si>
+    <t>AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTOR/ADDRESS_CONTRACTOR/…</t>
+  </si>
+  <si>
+    <t>hasEORole</t>
+  </si>
+  <si>
+    <t>EO Role Code</t>
+  </si>
+  <si>
+    <t>If AWARD_CONTRACT/AWARDED_CONTRACT/NO_AWARDED_TO_GROUP, then SC (Sole Contractor)</t>
+  </si>
+  <si>
+    <t>AWARD_CONTRACT/AWARDED_CONTRACT/@ITEM and LOT_NO (?)</t>
+  </si>
+  <si>
+    <t>regorg:RegisteredOrganization/EconomicOperator as Group</t>
+  </si>
+  <si>
+    <t>hasEOGroupCode</t>
+  </si>
+  <si>
+    <t>EO Group Code</t>
+  </si>
+  <si>
+    <t>If AWARD_CONTRACT/AWARDED_CONTRACT/AWARDED_TO_GROUP, then ?</t>
+  </si>
+  <si>
+    <t>TED does not carry information about the type of EO group</t>
+  </si>
+  <si>
+    <t>TED does not carry information about the type of EO role in the group</t>
   </si>
 </sst>
 </file>
@@ -1417,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,129 +1506,145 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>177</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>177</v>
+      <c r="B7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>150</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>4</v>
+        <v>220</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="135" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>79</v>
+        <v>147</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>71</v>
+        <v>161</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>6</v>
+        <v>148</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -1575,183 +1654,181 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="32" t="s">
-        <v>84</v>
+        <v>75</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>87</v>
+        <v>164</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>75</v>
+        <v>61</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="32" t="s">
+        <v>79</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>64</v>
+        <v>141</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D40" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="D43" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>151</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="B48" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
+    </row>
+    <row r="57" spans="4:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D57" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B51" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B52" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="D55" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B56" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>175</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="B2:D57">
+    <sortState ref="B3:D57">
+      <sortCondition ref="B2:B57"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="B2:B56">
     <sortCondition ref="B1"/>
   </sortState>
@@ -1762,10 +1839,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H57"/>
+  <dimension ref="B2:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:F38"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,18 +1870,18 @@
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="12" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -1815,10 +1892,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1826,10 +1903,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -1837,10 +1914,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1848,10 +1925,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -1859,10 +1936,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -1870,10 +1947,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -1881,10 +1958,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -1892,10 +1969,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -1903,10 +1980,10 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -1914,7 +1991,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>5</v>
@@ -1925,10 +2002,10 @@
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -1936,10 +2013,10 @@
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1947,7 +2024,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1989,13 +2066,13 @@
         <v>7</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="60" x14ac:dyDescent="0.25">
@@ -2003,16 +2080,16 @@
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="H24" s="25"/>
     </row>
@@ -2021,19 +2098,19 @@
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>41</v>
-      </c>
       <c r="F25" s="6" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="45" x14ac:dyDescent="0.25">
@@ -2041,19 +2118,19 @@
         <v>7</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="105" x14ac:dyDescent="0.25">
@@ -2061,19 +2138,19 @@
         <v>7</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="H27" s="21" t="s">
         <v>181</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="H27" s="21" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="45" x14ac:dyDescent="0.25">
@@ -2081,19 +2158,19 @@
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="60" x14ac:dyDescent="0.25">
@@ -2101,19 +2178,19 @@
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="120" x14ac:dyDescent="0.25">
@@ -2121,16 +2198,16 @@
         <v>7</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="H30" s="20"/>
     </row>
@@ -2139,13 +2216,13 @@
         <v>7</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="20"/>
@@ -2155,13 +2232,13 @@
         <v>7</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="20"/>
@@ -2171,13 +2248,13 @@
         <v>7</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="20"/>
@@ -2187,10 +2264,10 @@
         <v>7</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
@@ -2201,13 +2278,13 @@
         <v>7</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="20"/>
@@ -2217,13 +2294,13 @@
         <v>7</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="20"/>
@@ -2233,13 +2310,13 @@
         <v>7</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="20"/>
@@ -2251,7 +2328,7 @@
       <c r="C38" s="11"/>
       <c r="D38" s="4"/>
       <c r="F38" s="3" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="20"/>
@@ -2261,13 +2338,13 @@
         <v>7</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="20"/>
@@ -2277,13 +2354,13 @@
         <v>7</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="20"/>
@@ -2293,13 +2370,13 @@
         <v>7</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="20"/>
@@ -2309,13 +2386,13 @@
         <v>7</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="20"/>
@@ -2325,7 +2402,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
@@ -2338,10 +2415,10 @@
         <v>9</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
@@ -2349,10 +2426,10 @@
         <v>9</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
@@ -2360,18 +2437,18 @@
         <v>9</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="22" t="s">
-        <v>10</v>
+        <v>226</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
@@ -2381,16 +2458,16 @@
     </row>
     <row r="48" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>10</v>
+        <v>227</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>47</v>
+        <v>228</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>100</v>
+        <v>229</v>
+      </c>
+      <c r="F48" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -2398,13 +2475,13 @@
         <v>10</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>95</v>
+        <v>46</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
@@ -2412,13 +2489,13 @@
         <v>10</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>96</v>
+        <v>47</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
@@ -2426,24 +2503,27 @@
         <v>10</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>44</v>
+        <v>223</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2451,16 +2531,13 @@
         <v>10</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>97</v>
+        <v>239</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
@@ -2468,56 +2545,131 @@
         <v>10</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>76</v>
+        <v>51</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E56" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="F56" s="1" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>11</v>
+        <v>230</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>56</v>
+        <v>231</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>100</v>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2530,7 +2682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33:C44"/>
     </sheetView>
   </sheetViews>
@@ -2542,427 +2694,427 @@
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" t="s">
         <v>109</v>
       </c>
-      <c r="E2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="M2" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" t="s">
         <v>113</v>
       </c>
-      <c r="H2" t="s">
+      <c r="O2" t="s">
         <v>114</v>
       </c>
-      <c r="I2" t="s">
-        <v>115</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="P2" t="s">
         <v>116</v>
       </c>
-      <c r="K2" t="s">
+      <c r="Q2" t="s">
+        <v>117</v>
+      </c>
+      <c r="R2" t="s">
         <v>118</v>
       </c>
-      <c r="L2" t="s">
+      <c r="S2" t="s">
         <v>119</v>
       </c>
-      <c r="M2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N2" t="s">
-        <v>123</v>
-      </c>
-      <c r="O2" t="s">
-        <v>124</v>
-      </c>
-      <c r="P2" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>127</v>
-      </c>
-      <c r="R2" t="s">
-        <v>128</v>
-      </c>
-      <c r="S2" t="s">
-        <v>129</v>
-      </c>
       <c r="T2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="I3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="P3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="Q3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="R3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="J4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="K4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="L4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="N4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="O4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="I5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="J5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="K5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="L5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="M5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="N5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="O5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="P5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="Q5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="R5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="S5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="T5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="I6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="J6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="K6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="L6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="M6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="N6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="O6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="P6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="Q6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="R6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="S6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="T6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="I7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="K7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="P7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="Q7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="R7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="S7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="I8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="K8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="L8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="N8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="O8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="P8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="Q8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="R8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="S8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="T8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H9" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="N9" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="O9" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="P9" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="Q9" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="R9" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="T9" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L10" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="I11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="J11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="K11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="L11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="M11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="N11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="O11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="P11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="Q11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="R11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="S11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="T11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="M12" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="O13" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -2985,101 +3137,101 @@
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="P18" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="17"/>
       <c r="C19" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="P19" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="17"/>
       <c r="C20" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="17"/>
       <c r="P21" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="Q21" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="17"/>
       <c r="P22" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="Q22" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="F23" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="Q23" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
       <c r="F24" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="Q24" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="17"/>
       <c r="F25" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="17" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="I26" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="Q26" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="17"/>
       <c r="Q27" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="17"/>
       <c r="R28" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="17"/>
       <c r="R29" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
@@ -3131,104 +3283,104 @@
         <v>1</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C3" s="14"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C4" s="26"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C9" s="26"/>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C10" s="26"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C11" s="14"/>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C12" s="26"/>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C13" s="14"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C14" s="26"/>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C15" s="14"/>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C16" s="26"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="28" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C17" s="28"/>
     </row>

</xml_diff>

<commit_message>
Economic operator / winner mapping
</commit_message>
<xml_diff>
--- a/05_Implementation/PoC/Mapping TED XML to ePO.xlsx
+++ b/05_Implementation/PoC/Mapping TED XML to ePO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="250">
   <si>
     <t>ePO TTL</t>
   </si>
@@ -1851,7 +1851,7 @@
   <dimension ref="B2:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2641,6 +2641,9 @@
       <c r="F58" s="3" t="s">
         <v>235</v>
       </c>
+      <c r="G58" s="1" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
@@ -2655,6 +2658,9 @@
       <c r="F59" s="3" t="s">
         <v>238</v>
       </c>
+      <c r="G59" s="1" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
@@ -2668,6 +2674,9 @@
       </c>
       <c r="F60" s="3" t="s">
         <v>222</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="61" spans="2:8" ht="30" x14ac:dyDescent="0.25">

</xml_diff>